<commit_message>
Season 13, Matchday 9
</commit_message>
<xml_diff>
--- a/data/bombs_2.xlsx
+++ b/data/bombs_2.xlsx
@@ -1,20 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton.shevchuk\dev\euroleague\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0949DDC-E80A-494D-BDD2-EE2DC342CDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="52">
   <si>
     <t>Бомбардир</t>
   </si>
@@ -97,9 +114,6 @@
     <t>бонгонда (генк)</t>
   </si>
   <si>
-    <t>линссен (фейнорд)</t>
-  </si>
-  <si>
     <t>белотти (торино)</t>
   </si>
   <si>
@@ -124,24 +138,12 @@
     <t>влахович (фиорентина)</t>
   </si>
   <si>
-    <t>кэлверт-льюин (эвертон)</t>
-  </si>
-  <si>
-    <t>тиль (фейе)</t>
-  </si>
-  <si>
     <t>версарен (андерлехт)</t>
   </si>
   <si>
-    <t>лукаку(челси)</t>
-  </si>
-  <si>
     <t>смолов (локомотив)</t>
   </si>
   <si>
-    <t>салах(ливерпуль)</t>
-  </si>
-  <si>
     <t>дессерс (генк)</t>
   </si>
   <si>
@@ -169,53 +171,29 @@
     <t>де томас (эспаньол)</t>
   </si>
   <si>
-    <t>смолов (локо)</t>
-  </si>
-  <si>
-    <t>ричарлисон (эвертон)</t>
-  </si>
-  <si>
     <t>нкунку (лейпциг)</t>
   </si>
   <si>
-    <t>сен максимен (ньюкасл)</t>
-  </si>
-  <si>
-    <t>линссен(фейнорд)</t>
-  </si>
-  <si>
-    <t>белоти(торино)</t>
-  </si>
-  <si>
     <t>андре силва (рб лейпциг)</t>
   </si>
   <si>
-    <t>белоти (торино)</t>
-  </si>
-  <si>
     <t>собослаи (рб лейпциг)</t>
   </si>
   <si>
-    <t>кальверт-льюин (эвертон)</t>
-  </si>
-  <si>
     <t>силва (лейпциг)</t>
   </si>
   <si>
     <t>аль-гаддиуи (штутгарт)</t>
   </si>
   <si>
-    <t>силва (рб)</t>
-  </si>
-  <si>
-    <t>линсен (фейеноорд)</t>
+    <t>сен-максимен (ньюкасл)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +256,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -324,7 +310,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -356,9 +342,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,6 +394,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -565,14 +587,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -580,39 +608,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -620,15 +648,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -636,503 +664,482 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B43" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B48" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B49" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B53" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B56" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B57" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B58" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B59" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B60" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B61" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B63" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B64" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B65" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B66" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B67" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B68" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B69" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B70" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B67">
+    <sortCondition ref="A20:A67"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>